<commit_message>
examples: updated excel imports example start payroll: added regulation excel with json convert updated version to 0.9.0-beta.8
</commit_message>
<xml_diff>
--- a/Examples/TimesheetPayroll/Case.Data/WorkTimes.2025.Week8.xlsx
+++ b/Examples/TimesheetPayroll/Case.Data/WorkTimes.2025.Week8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\Examples\TimesheetPayroll\Case.Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF924EF7-BDBC-4986-B5A8-C55B46D730AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF93F453-7BA4-4A76-A14C-1658B34B89AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,51 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -373,6 +417,20 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Ioannis Giannoudis" id="{D72C8328-3D44-4E24-B9E6-5B2C39CC71AE}" userId="f6c6fce19d9413b9" providerId="Windows Live"/>
 </personList>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3729C50A-E874-4135-8C3F-31B6A5647FEB}" name="Table1" displayName="Table1" ref="A2:F6" headerRowCount="0" totalsRowShown="0" dataDxfId="5">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E1215DE4-854A-49AA-9BF2-A4F4E36921FB}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{D778E6FE-F2E9-4DD5-8566-15FF85B3FEDC}" name="Column2" headerRowDxfId="0" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{3E04550D-860B-4B85-B66B-4BC5A7DC9F20}" name="Column3" headerRowDxfId="1" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{4683801D-6CD1-4F1E-98F9-FE17003F6C27}" name="Column4" headerRowDxfId="2" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{D382A701-D7F1-4EE1-BD87-3834C4431B09}" name="Column5" headerRowDxfId="3" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{92BAA078-3F98-4DAD-BE3E-1F7791DC48D0}" name="Column6" headerRowDxfId="4" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,24 +733,24 @@
   </sheetPr>
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="2.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="8.5500000000000007" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
@@ -704,7 +762,7 @@
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
@@ -712,7 +770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -720,7 +778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -728,7 +786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
@@ -736,7 +794,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -744,7 +802,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
@@ -752,12 +810,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
@@ -771,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
@@ -781,7 +839,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="6"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" s="8" t="s">
         <v>4</v>
       </c>
@@ -795,7 +853,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
@@ -809,7 +867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -823,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
         <v>27</v>
       </c>
@@ -853,23 +911,23 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:F187"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="12" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" style="13" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="20.6328125" style="12" customWidth="1"/>
+    <col min="2" max="3" width="15.6328125" style="13" customWidth="1"/>
+    <col min="4" max="5" width="15.6328125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>31</v>
       </c>
@@ -889,7 +947,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -909,7 +967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -929,7 +987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -949,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -969,7 +1027,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -989,187 +1047,186 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <hyperlinks>
@@ -1181,5 +1238,8 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
+  <tableParts count="1">
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>